<commit_message>
Cleaning ver data sheets
</commit_message>
<xml_diff>
--- a/notebooks/mkappa/verification_data/Rem20/Abbildung_4-12/rem18_4-12-a.xlsx
+++ b/notebooks/mkappa/verification_data/Rem20/Abbildung_4-12/rem18_4-12-a.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IMB\PyCharm_workspace\bmcs_cross_section\notebooks\mkappa\verification_data\Rem20\Abbildung_4-12\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IMB\PyCharm_workspace\bmcs_cross_section\notebooks\mkappa\verification_data\rem20\Abbildung_4-12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAFD2BA5-B2C3-477A-B1B1-80BA75DFD6DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D764A2C8-D6B7-4994-9D4E-D5C39E34C0C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3020" yWindow="1420" windowWidth="10800" windowHeight="8780" xr2:uid="{EF743041-95B4-491C-8AF6-66DDE6754244}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{EF743041-95B4-491C-8AF6-66DDE6754244}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -401,10 +401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85653E29-E61E-4045-870B-179DFE103CEF}">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -413,441 +413,413 @@
     <col min="2" max="2" width="10.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
       </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
       <c r="D1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" s="1">
         <v>0</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
       <c r="D2" s="1">
         <v>0</v>
       </c>
-      <c r="E2" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>5.1282051282051282E-3</v>
       </c>
       <c r="B3" s="1">
         <v>0.1388888888888889</v>
       </c>
-      <c r="C3" s="2"/>
+      <c r="C3" s="1">
+        <v>1.0256410256410256E-2</v>
+      </c>
       <c r="D3" s="1">
-        <v>1.0256410256410256E-2</v>
-      </c>
-      <c r="E3" s="1">
         <v>0.85648148148148151</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>7.6923076923076919E-3</v>
       </c>
       <c r="B4" s="1">
         <v>0.25462962962962959</v>
       </c>
-      <c r="C4" s="2"/>
+      <c r="C4" s="1">
+        <v>2.3076923076923078E-2</v>
+      </c>
       <c r="D4" s="1">
-        <v>2.3076923076923078E-2</v>
-      </c>
-      <c r="E4" s="1">
         <v>0.87962962962962965</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>1.282051282051282E-2</v>
       </c>
       <c r="B5" s="1">
         <v>0.25462962962962959</v>
       </c>
-      <c r="C5" s="2"/>
+      <c r="C5" s="1">
+        <v>3.0769230769230767E-2</v>
+      </c>
       <c r="D5" s="1">
-        <v>3.0769230769230767E-2</v>
-      </c>
-      <c r="E5" s="1">
         <v>0.87962962962962965</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>3.8461538461538457E-2</v>
       </c>
       <c r="B6" s="1">
         <v>0.35879629629629628</v>
       </c>
-      <c r="C6" s="2"/>
+      <c r="C6" s="1">
+        <v>4.8717948717948718E-2</v>
+      </c>
       <c r="D6" s="1">
-        <v>4.8717948717948718E-2</v>
-      </c>
-      <c r="E6" s="1">
         <v>1.0069444444444444</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>4.6153846153846156E-2</v>
       </c>
       <c r="B7" s="1">
         <v>0.34722222222222221</v>
       </c>
-      <c r="C7" s="2"/>
+      <c r="C7" s="1">
+        <v>6.4102564102564097E-2</v>
+      </c>
       <c r="D7" s="1">
-        <v>6.4102564102564097E-2</v>
-      </c>
-      <c r="E7" s="1">
         <v>1.0416666666666667</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>5.128205128205128E-2</v>
       </c>
       <c r="B8" s="1">
         <v>0.32407407407407407</v>
       </c>
-      <c r="C8" s="2"/>
+      <c r="C8" s="1">
+        <v>6.9230769230769235E-2</v>
+      </c>
       <c r="D8" s="1">
-        <v>6.9230769230769235E-2</v>
-      </c>
-      <c r="E8" s="1">
         <v>1.0763888888888888</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>6.1538461538461535E-2</v>
       </c>
       <c r="B9" s="1">
         <v>0.3125</v>
       </c>
-      <c r="C9" s="2"/>
+      <c r="C9" s="1">
+        <v>7.9487179487179482E-2</v>
+      </c>
       <c r="D9" s="1">
-        <v>7.9487179487179482E-2</v>
-      </c>
-      <c r="E9" s="1">
         <v>1.2152777777777777</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>8.4615384615384606E-2</v>
       </c>
       <c r="B10" s="1">
         <v>0.41666666666666663</v>
       </c>
-      <c r="C10" s="2"/>
+      <c r="C10" s="1">
+        <v>9.2307692307692313E-2</v>
+      </c>
       <c r="D10" s="1">
-        <v>9.2307692307692313E-2</v>
-      </c>
-      <c r="E10" s="1">
         <v>1.1689814814814816</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>0.10256410256410256</v>
       </c>
       <c r="B11" s="1">
         <v>0.41666666666666663</v>
       </c>
-      <c r="C11" s="2"/>
+      <c r="C11" s="1">
+        <v>9.9999999999999992E-2</v>
+      </c>
       <c r="D11" s="1">
-        <v>9.9999999999999992E-2</v>
-      </c>
-      <c r="E11" s="1">
         <v>1.2152777777777777</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>0.11025641025641027</v>
       </c>
       <c r="B12" s="1">
         <v>0.3125</v>
       </c>
-      <c r="C12" s="2"/>
+      <c r="C12" s="1">
+        <v>0.10769230769230768</v>
+      </c>
       <c r="D12" s="1">
-        <v>0.10769230769230768</v>
-      </c>
-      <c r="E12" s="1">
         <v>1.3425925925925928</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>0.12051282051282051</v>
       </c>
       <c r="B13" s="1">
         <v>0.38194444444444448</v>
       </c>
-      <c r="C13" s="2"/>
+      <c r="C13" s="1">
+        <v>0.12307692307692307</v>
+      </c>
       <c r="D13" s="1">
-        <v>0.12307692307692307</v>
-      </c>
-      <c r="E13" s="1">
         <v>1.400462962962963</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>0.13076923076923078</v>
       </c>
       <c r="B14" s="1">
         <v>0.41666666666666663</v>
       </c>
-      <c r="C14" s="2"/>
+      <c r="C14" s="1">
+        <v>0.13076923076923078</v>
+      </c>
       <c r="D14" s="1">
-        <v>0.13076923076923078</v>
-      </c>
-      <c r="E14" s="1">
         <v>1.4814814814814814</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>0.14871794871794872</v>
       </c>
       <c r="B15" s="1">
         <v>0.4513888888888889</v>
       </c>
-      <c r="C15" s="2"/>
+      <c r="C15" s="1">
+        <v>0.14358974358974358</v>
+      </c>
       <c r="D15" s="1">
-        <v>0.14358974358974358</v>
-      </c>
-      <c r="E15" s="1">
         <v>1.5393518518518516</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>0.16153846153846152</v>
       </c>
       <c r="B16" s="1">
         <v>0.38194444444444448</v>
       </c>
-      <c r="C16" s="2"/>
+      <c r="C16" s="1">
+        <v>0.15897435897435896</v>
+      </c>
       <c r="D16" s="1">
-        <v>0.15897435897435896</v>
-      </c>
-      <c r="E16" s="1">
         <v>1.6203703703703702</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>0.18974358974358974</v>
       </c>
       <c r="B17" s="1">
         <v>0.43981481481481483</v>
       </c>
-      <c r="C17" s="2"/>
+      <c r="C17" s="1">
+        <v>0.16666666666666666</v>
+      </c>
       <c r="D17" s="1">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="E17" s="1">
         <v>1.7013888888888888</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>0.20769230769230768</v>
       </c>
       <c r="B18" s="1">
         <v>0.41666666666666663</v>
       </c>
-      <c r="C18" s="2"/>
+      <c r="C18" s="1">
+        <v>0.17179487179487177</v>
+      </c>
       <c r="D18" s="1">
-        <v>0.17179487179487177</v>
-      </c>
-      <c r="E18" s="1">
         <v>1.724537037037037</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>0.22051282051282053</v>
       </c>
       <c r="B19" s="1">
         <v>0.40509259259259256</v>
       </c>
-      <c r="C19" s="2"/>
+      <c r="C19" s="1">
+        <v>0.17948717948717949</v>
+      </c>
       <c r="D19" s="1">
-        <v>0.17948717948717949</v>
-      </c>
-      <c r="E19" s="1">
         <v>1.724537037037037</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>0.24358974358974358</v>
       </c>
       <c r="B20" s="1">
         <v>0.47453703703703709</v>
       </c>
-      <c r="C20" s="2"/>
+      <c r="C20" s="1">
+        <v>0.19999999999999998</v>
+      </c>
       <c r="D20" s="1">
-        <v>0.19999999999999998</v>
-      </c>
-      <c r="E20" s="1">
         <v>1.8634259259259258</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>0.26153846153846155</v>
       </c>
       <c r="B21" s="1">
         <v>0.46296296296296291</v>
       </c>
-      <c r="C21" s="2"/>
+      <c r="C21" s="1">
+        <v>0.21538461538461537</v>
+      </c>
       <c r="D21" s="1">
-        <v>0.21538461538461537</v>
-      </c>
-      <c r="E21" s="1">
         <v>1.9907407407407407</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>0.29230769230769227</v>
       </c>
       <c r="B22" s="1">
         <v>0.52083333333333337</v>
       </c>
-      <c r="C22" s="2"/>
+      <c r="C22" s="1">
+        <v>0.22820512820512817</v>
+      </c>
       <c r="D22" s="1">
-        <v>0.22820512820512817</v>
-      </c>
-      <c r="E22" s="1">
         <v>2.0717592592592595</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>0.31025641025641026</v>
       </c>
       <c r="B23" s="1">
         <v>0.49768518518518517</v>
       </c>
-      <c r="C23" s="2"/>
+      <c r="C23" s="1">
+        <v>0.24102564102564103</v>
+      </c>
       <c r="D23" s="1">
-        <v>0.24102564102564103</v>
-      </c>
-      <c r="E23" s="1">
         <v>2.1180555555555554</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>0.32564102564102559</v>
       </c>
       <c r="B24" s="1">
         <v>0.52083333333333337</v>
       </c>
-      <c r="C24" s="2"/>
+      <c r="C24" s="1">
+        <v>0.24871794871794872</v>
+      </c>
       <c r="D24" s="1">
-        <v>0.24871794871794872</v>
-      </c>
-      <c r="E24" s="1">
         <v>2.1296296296296298</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>0.34102564102564098</v>
       </c>
       <c r="B25" s="1">
         <v>0.56712962962962965</v>
       </c>
-      <c r="C25" s="2"/>
+      <c r="C25" s="1">
+        <v>0.258974358974359</v>
+      </c>
       <c r="D25" s="1">
-        <v>0.258974358974359</v>
-      </c>
-      <c r="E25" s="1">
         <v>2.1875</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>0.35128205128205131</v>
       </c>
       <c r="B26" s="1">
         <v>0.56712962962962965</v>
       </c>
-      <c r="C26" s="2"/>
+      <c r="C26" s="1">
+        <v>0.26666666666666666</v>
+      </c>
       <c r="D26" s="1">
-        <v>0.26666666666666666</v>
-      </c>
-      <c r="E26" s="1">
         <v>2.2453703703703702</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>0.37692307692307692</v>
       </c>
       <c r="B27" s="1">
         <v>0.60185185185185186</v>
       </c>
-      <c r="C27" s="2"/>
+      <c r="C27" s="1">
+        <v>0.27179487179487177</v>
+      </c>
       <c r="D27" s="1">
-        <v>0.27179487179487177</v>
-      </c>
-      <c r="E27" s="1">
         <v>2.2800925925925926</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>0.39999999999999997</v>
       </c>
       <c r="B28" s="1">
         <v>0.61342592592592593</v>
       </c>
-      <c r="C28" s="2"/>
+      <c r="C28" s="1">
+        <v>0.27948717948717949</v>
+      </c>
       <c r="D28" s="1">
-        <v>0.27948717948717949</v>
-      </c>
-      <c r="E28" s="1">
         <v>2.3379629629629632</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>0.41025641025641024</v>
       </c>
       <c r="B29" s="1">
         <v>0.60185185185185186</v>
       </c>
-      <c r="C29" s="2"/>
+      <c r="C29" s="1">
+        <v>0.29487179487179482</v>
+      </c>
       <c r="D29" s="1">
-        <v>0.29487179487179482</v>
-      </c>
-      <c r="E29" s="1">
         <v>2.3263888888888888</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>0.42820512820512818</v>
       </c>
@@ -856,9 +828,8 @@
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>0.44102564102564107</v>
       </c>
@@ -867,9 +838,8 @@
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>0.4589743589743589</v>
       </c>
@@ -878,9 +848,8 @@
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>0.50512820512820511</v>
       </c>
@@ -889,9 +858,8 @@
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>0.53333333333333333</v>
       </c>
@@ -900,9 +868,8 @@
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>0.56923076923076921</v>
       </c>
@@ -911,9 +878,8 @@
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>0.58461538461538454</v>
       </c>
@@ -922,9 +888,8 @@
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>0.6102564102564102</v>
       </c>
@@ -933,9 +898,8 @@
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>0.62051282051282053</v>
       </c>
@@ -944,9 +908,8 @@
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>0.63589743589743586</v>
       </c>
@@ -955,9 +918,8 @@
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>0.65384615384615374</v>
       </c>
@@ -966,9 +928,8 @@
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>0.67435897435897429</v>
       </c>
@@ -977,9 +938,8 @@
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>0.69230769230769218</v>
       </c>
@@ -988,7 +948,6 @@
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>